<commit_message>
Retoque de requerimientos, primera idea de cronograma
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -63,9 +68,6 @@
     <t>Creación de grupo foco usuarios, creación de encuesta general para usuarios. Busqueda de aplicaciones del mismo estilo (Bicos-Brasil y Calificados-Argentina)</t>
   </si>
   <si>
-    <t>Alto</t>
-  </si>
-  <si>
     <t>Riesgos</t>
   </si>
   <si>
@@ -82,6 +84,9 @@
   </si>
   <si>
     <t>Creación de grupo foco usuarios, creación de encuesta general para usuarios.</t>
+  </si>
+  <si>
+    <t>Requerimientos. Mayor detalle, estimación de tiempo. Cronograma primera idea</t>
   </si>
 </sst>
 </file>
@@ -420,7 +425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -428,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,9 +491,6 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -588,7 +590,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1">
         <v>42835</v>
@@ -600,7 +602,7 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -634,7 +636,7 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -651,7 +653,7 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -668,7 +670,7 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -685,7 +687,24 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1">
+        <v>42842</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retoques Anteproyecto. Gantt (sin entregables, hitos)
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Cronograma</t>
+  </si>
+  <si>
+    <t>Investigación</t>
+  </si>
+  <si>
+    <t>Angular</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,6 +733,40 @@
         <v>21</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <v>42844</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>42845</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Estudio de alternativas. Anteproyecto
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="27">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Angular</t>
+  </si>
+  <si>
+    <t>Retoques Anteproyecto, gráfico de Gantt</t>
+  </si>
+  <si>
+    <t>Retoques Anteproyecto, Estudio de alternativas</t>
+  </si>
+  <si>
+    <t>Video tutorial Angular 2</t>
   </si>
 </sst>
 </file>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,6 +776,57 @@
         <v>23</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1">
+        <v>42849</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1">
+        <v>42850</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>42851</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Avanzando con el MER. Se dejó una verisón inicial sin atributos. Un Word con los atributos detallados, consultas para realizar y detalles a ver entre nosotros. Cuando tengamos una versión definitiva del MER, recién ahí le agregamos los atributos, sino es imposible trabajarlo con todas las flechas saliendo de las entidades.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -459,7 +459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -467,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,6 +996,23 @@
         <v>33</v>
       </c>
     </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="1">
+        <v>42862</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Armado de primera idea de Diagrama de clases genereal. Realización de diagrama de clases de primer Sprint. Armado de las capas y estructura en c#. Interfaz del servicio realizada con una prueba en consola para testear funcionalidad
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -121,6 +126,18 @@
   </si>
   <si>
     <t>Modificando el MER a partir de la lista de requerimientos</t>
+  </si>
+  <si>
+    <t>Sprint 1 - Diagrama de Clases</t>
+  </si>
+  <si>
+    <t>Idea general de Diagrama de clases, creación de Diagrama de clases para Sprint1</t>
+  </si>
+  <si>
+    <t>Sprint 1 - Back-end</t>
+  </si>
+  <si>
+    <t>Armado de las capas y estructura del back-end, investigación de servicios web, realización de la interfas del servicio.</t>
   </si>
 </sst>
 </file>
@@ -459,7 +476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -467,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1013,6 +1030,40 @@
         <v>33</v>
       </c>
     </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1">
+        <v>42863</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1">
+        <v>42864</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Retoques en las firmas de la interfaz de servicio. Actualización del diagrama UML
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -487,7 +487,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,7 +1055,7 @@
         <v>42864</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Script DB, Proyecto ANGULAR
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="43">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -119,9 +114,6 @@
     <t>Arreglos</t>
   </si>
   <si>
-    <t>Sprint 1 - MER</t>
-  </si>
-  <si>
     <t>Agregando atributos y Entidades al MER</t>
   </si>
   <si>
@@ -141,6 +133,21 @@
   </si>
   <si>
     <t>Validaciones en la capa de logica, creación de la capa de testing, realización de una prueba sobre el servicio para probar funcionamiento</t>
+  </si>
+  <si>
+    <t>Modificando el MER a partir de la lista de requerimientos (Con ayuda de Fernando)</t>
+  </si>
+  <si>
+    <t>Posible MER final - Pasaje a MR - Comienzo de creación de Script</t>
+  </si>
+  <si>
+    <t>Sprint 3 - FrontEnd</t>
+  </si>
+  <si>
+    <t>Sprint 3 - Base de Datos</t>
+  </si>
+  <si>
+    <t>Copiado de Proyecto de Angular para crear esqueleto - Verificación de que el proyecto corra tal y como estaba para poder realizarle cambios</t>
   </si>
 </sst>
 </file>
@@ -479,7 +486,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -487,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,10 +1000,10 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" t="s">
         <v>31</v>
-      </c>
-      <c r="E30" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1010,10 +1017,10 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1027,10 +1034,10 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1044,10 +1051,10 @@
         <v>3</v>
       </c>
       <c r="D33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" t="s">
         <v>34</v>
-      </c>
-      <c r="E33" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1061,10 +1068,10 @@
         <v>7</v>
       </c>
       <c r="D34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" t="s">
         <v>36</v>
-      </c>
-      <c r="E34" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1078,10 +1085,78 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="1">
+        <v>42865</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="1">
+        <v>42865</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="1">
+        <v>42868</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="1">
+        <v>42868</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed en FrontEnd, Registro de hora de trabajo.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="45">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -156,6 +151,9 @@
   </si>
   <si>
     <t>Comienzo de Front-end</t>
+  </si>
+  <si>
+    <t>Borrado de componentes no no utilizados.</t>
   </si>
 </sst>
 </file>
@@ -494,7 +492,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -502,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,6 +1199,23 @@
         <v>43</v>
       </c>
     </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="1">
+        <v>42869</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Alta Cliente y Actualizar Cliente Back-end prontos
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="47">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -120,15 +125,9 @@
     <t>Modificando el MER a partir de la lista de requerimientos</t>
   </si>
   <si>
-    <t>Sprint 1 - Diagrama de Clases</t>
-  </si>
-  <si>
     <t>Idea general de Diagrama de clases, creación de Diagrama de clases para Sprint1</t>
   </si>
   <si>
-    <t>Sprint 1 - Back-end</t>
-  </si>
-  <si>
     <t>Armado de las capas y estructura del back-end, investigación de servicios web, realización de la interfas del servicio.</t>
   </si>
   <si>
@@ -154,6 +153,18 @@
   </si>
   <si>
     <t>Borrado de componentes no no utilizados.</t>
+  </si>
+  <si>
+    <t>Sprint 3 - Diagrama de Clases</t>
+  </si>
+  <si>
+    <t>Sprint 3 - Back-end</t>
+  </si>
+  <si>
+    <t>Sprint 3 - BackEnd</t>
+  </si>
+  <si>
+    <t>Conexión a la BD, alta cliente</t>
   </si>
 </sst>
 </file>
@@ -492,7 +503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1006,7 +1017,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E30" t="s">
         <v>31</v>
@@ -1023,7 +1034,7 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E31" t="s">
         <v>32</v>
@@ -1040,7 +1051,7 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E32" t="s">
         <v>32</v>
@@ -1057,10 +1068,10 @@
         <v>3</v>
       </c>
       <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
         <v>33</v>
-      </c>
-      <c r="E33" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1074,10 +1085,10 @@
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1091,10 +1102,10 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" t="s">
         <v>35</v>
-      </c>
-      <c r="E35" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1108,7 +1119,7 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E36" t="s">
         <v>32</v>
@@ -1125,10 +1136,10 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1142,10 +1153,10 @@
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1159,10 +1170,10 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" t="s">
         <v>40</v>
-      </c>
-      <c r="E39" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1176,10 +1187,10 @@
         <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1193,10 +1204,10 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1210,10 +1221,27 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E42" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1">
+        <v>42870</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alta Cliente, Actualizar Cliente, Actualizar Contrase;a, Obtener todos los cliente. Testeado desde consola. Tirando la base y ejecutando de nuevo el script, se pueden realizar las pruebas de la consola.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="48">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Conexión a la BD, alta cliente</t>
+  </si>
+  <si>
+    <t>Alta Cliente, Actualizar Cliente, Actualizar Contrase;a, Obtener todos los clientes</t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,6 +1247,23 @@
         <v>46</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="1">
+        <v>42871</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Back-end Cliente y Administrador casi pronto
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="49">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Alta Cliente, Actualizar Cliente, Actualizar Contrase;a, Obtener todos los clientes</t>
+  </si>
+  <si>
+    <t>Ingreso Cliente, Todo el Backend Administrador</t>
   </si>
 </sst>
 </file>
@@ -514,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,6 +1267,23 @@
         <v>47</v>
       </c>
     </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1">
+        <v>42872</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Integración Back-Front - Pruebas con API REST
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="52">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -171,6 +166,15 @@
   </si>
   <si>
     <t>Ingreso Cliente, Todo el Backend Administrador</t>
+  </si>
+  <si>
+    <t>Sprint 3 - Integración BackEnd y FrontEnd</t>
+  </si>
+  <si>
+    <t>Familiarización son lo creado por Federico</t>
+  </si>
+  <si>
+    <t>Investigación sobre API REST</t>
   </si>
 </sst>
 </file>
@@ -509,7 +513,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -517,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1284,6 +1288,57 @@
         <v>48</v>
       </c>
     </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="1">
+        <v>42878</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="1">
+        <v>42878</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="1">
+        <v>42879</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Subo donde deje no es nada pero da para probar y ver el error que tira. Esta cambiado lo de las rutas para acceder con el nombre del metodo anda en FireFox
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="52">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -513,7 +518,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -521,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1339,6 +1344,40 @@
         <v>51</v>
       </c>
     </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="1">
+        <v>42879</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="1">
+        <v>42880</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Integración BackEnd y FrontEnd andando... Subo para poder seguir probando hasta tener algún servicio un poco más complejo andando... Después, es copiar y pegar...
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -180,6 +175,9 @@
   </si>
   <si>
     <t>Investigación sobre API REST</t>
+  </si>
+  <si>
+    <t>Investigación sobre API REST - Servicios del back ya responden al llamarlos desde el front</t>
   </si>
 </sst>
 </file>
@@ -518,7 +516,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -526,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1378,6 +1376,23 @@
         <v>51</v>
       </c>
     </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="1">
+        <v>42881</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Trabajando con objetos dentro de objetos en los servicios. Funciona OK. Quedan estos ejemplos de muestra...
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="55">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>Investigación sobre API REST - Servicios del back ya responden al llamarlos desde el front</t>
+  </si>
+  <si>
+    <t>Se crearon 5 ejemplos de llamadas a servicios (1 DELETE, 1 POST, 1 PUT, 2 GET -Uno con y uno sin parámetro-)</t>
+  </si>
+  <si>
+    <t>Se modificaron lo 5 ejemplos para pasar a trabajar con objetos dentro de objetos.</t>
   </si>
 </sst>
 </file>
@@ -516,7 +522,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1393,6 +1399,40 @@
         <v>52</v>
       </c>
     </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="1">
+        <v>42882</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="1">
+        <v>42882</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modificación en los servicios del cliente, cambios en la visual del front (eliminé todo lo no responsivo), eliminación de todo lo que no era de nuestro proyecto
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="59">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>Se modificaron lo 5 ejemplos para pasar a trabajar con objetos dentro de objetos.</t>
+  </si>
+  <si>
+    <t>Pruebas con servicios nuestros (Servicios del Cliente) para implementar soluciones genéricas</t>
+  </si>
+  <si>
+    <t>Eliminación de todo lo que tenía que ver con MARPH del proyecto del Front</t>
+  </si>
+  <si>
+    <t>Eliminación de todo aspecto que no fuera reponsivo (por si implementamos app mobile)</t>
+  </si>
+  <si>
+    <t>Investigación sobre Token en .NET (No llegué a ninguna conclusión interesante… Vi alguna forma de crear nuestro propio token)</t>
   </si>
 </sst>
 </file>
@@ -522,7 +534,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -530,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1433,6 +1445,91 @@
         <v>54</v>
       </c>
     </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="1">
+        <v>42882</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="1">
+        <v>42883</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="1">
+        <v>42883</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="1">
+        <v>42883</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="1">
+        <v>42883</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>49</v>
+      </c>
+      <c r="E58" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Front cliente casi terminado, falta realizar controles de seguridad. Llave de acceso, rederigir paginas si no estas logueado, borrar local storage al cerrar sesion
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="61">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -196,6 +201,12 @@
   </si>
   <si>
     <t>Investigación sobre Token en .NET (No llegué a ninguna conclusión interesante… Vi alguna forma de crear nuestro propio token)</t>
+  </si>
+  <si>
+    <t>Lectura de lo realizado por Bruno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alta Cliente e ingreso de cliente </t>
   </si>
 </sst>
 </file>
@@ -534,7 +545,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1530,6 +1541,40 @@
         <v>55</v>
       </c>
     </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="1">
+        <v>42883</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="1">
+        <v>42884</v>
+      </c>
+      <c r="C60">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>49</v>
+      </c>
+      <c r="E60" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Administrador Front - En contrucci'on
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="63">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t xml:space="preserve">Alta Cliente e ingreso de cliente </t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Sprint 3 - BackEnd y FrontEnd</t>
   </si>
 </sst>
 </file>
@@ -553,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1575,6 +1581,40 @@
         <v>60</v>
       </c>
     </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="1">
+        <v>42885</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61" t="s">
+        <v>62</v>
+      </c>
+      <c r="E61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="1">
+        <v>42892</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62" t="s">
+        <v>62</v>
+      </c>
+      <c r="E62" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Front Administrador- casi todo pronto, falta imagenes en los clientes y administradores, en caso de querer tambien faltaría que los administradores editaran los datos de los clientes (cambio de contrase;a en caso de perdida y datos comunes).
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1606,7 +1606,7 @@
         <v>42892</v>
       </c>
       <c r="C62">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D62" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Administrador - Arreglos en funcionalidades. Algunas Pruebas IU cliente y administrador. Todo pronto la parte de administrador y superAdministrador
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="64">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Sprint 3 - BackEnd y FrontEnd</t>
+  </si>
+  <si>
+    <t>Administrador - Arreglos en funcionalidades. Algunas Pruebas IU cliente y administrador</t>
   </si>
 </sst>
 </file>
@@ -559,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1615,6 +1618,23 @@
         <v>61</v>
       </c>
     </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="1">
+        <v>42893</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>38</v>
+      </c>
+      <c r="E63" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Trabajando en testing WebAPI
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="66">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>Administrador - Arreglos en funcionalidades. Algunas Pruebas IU cliente y administrador</t>
+  </si>
+  <si>
+    <t>Sprint 3 - Testing</t>
+  </si>
+  <si>
+    <t>Testing WebAPI</t>
   </si>
 </sst>
 </file>
@@ -251,9 +257,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1626,7 +1633,7 @@
         <v>42893</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D63" t="s">
         <v>38</v>
@@ -1635,7 +1642,28 @@
         <v>63</v>
       </c>
     </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="1">
+        <v>42894</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>64</v>
+      </c>
+      <c r="E64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D65" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Subo solo las horas metidas hasta ahora, no quiero cagar todo el código y estoy tocando de todo para hacer pruebas. Por ahora, no llegué a nada que valga la pena. Cuando consiga un ejemplo andando subo solo eso!
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="72">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -222,6 +217,24 @@
   </si>
   <si>
     <t>Testing WebAPI</t>
+  </si>
+  <si>
+    <t>Sprint 3 - Investigación</t>
+  </si>
+  <si>
+    <t>Investigación sobre autenticación y lectura de documentación de proyectos (Sprints 3 y 4)</t>
+  </si>
+  <si>
+    <t>Investigación sobre animación de carga de datos en cada servicio</t>
+  </si>
+  <si>
+    <t>Investigación de pantalla de carga inicial</t>
+  </si>
+  <si>
+    <t>Investigación sobre autenticación</t>
+  </si>
+  <si>
+    <t>Investigación sobre subida de imágenes</t>
   </si>
 </sst>
 </file>
@@ -257,10 +270,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,7 +573,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -569,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1610,57 +1622,139 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B62" s="1">
-        <v>42892</v>
+        <v>42889</v>
       </c>
       <c r="C62">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D62" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E62" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B63" s="1">
-        <v>42893</v>
+        <v>42889</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="E63" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B64" s="1">
+        <v>42890</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>66</v>
+      </c>
+      <c r="E64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" s="1">
+        <v>42890</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65" t="s">
+        <v>66</v>
+      </c>
+      <c r="E65" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="1">
+        <v>42892</v>
+      </c>
+      <c r="C66">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
+        <v>62</v>
+      </c>
+      <c r="E66" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" s="1">
+        <v>42893</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>38</v>
+      </c>
+      <c r="E67" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="1">
         <v>42894</v>
       </c>
-      <c r="C64">
+      <c r="C68">
         <v>3</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D68" t="s">
         <v>64</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E68" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D65" s="2"/>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" s="1">
+        <v>42895</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>66</v>
+      </c>
+      <c r="E69" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Subo solo el registro de horas y el excel con la idea de la base de datos. No subo el código porque lo tengo hecho pedazos de hacer pruebas. No quiero borrar nada por ahora porque cada vez me siento más cerca de lograr algo con las imágenes jaja.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="75">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>Investigación sobre subida de imágenes</t>
+  </si>
+  <si>
+    <t>Pruebas para realizar la subida de imágenes</t>
+  </si>
+  <si>
+    <t>Sprint 4 - Base de Datos</t>
+  </si>
+  <si>
+    <t>Análisis de Base de Datos para incorporación de Sprint</t>
   </si>
 </sst>
 </file>
@@ -581,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E1090"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1756,6 +1765,3111 @@
         <v>71</v>
       </c>
     </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70" s="1">
+        <v>42896</v>
+      </c>
+      <c r="C70">
+        <v>7</v>
+      </c>
+      <c r="D70" t="s">
+        <v>66</v>
+      </c>
+      <c r="E70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" s="1">
+        <v>42897</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>66</v>
+      </c>
+      <c r="E71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" s="1">
+        <v>42897</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72" t="s">
+        <v>73</v>
+      </c>
+      <c r="E72" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B106" s="1"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B107" s="1"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B108" s="1"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B109" s="1"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" s="1"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B111" s="1"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B113" s="1"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B114" s="1"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B115" s="1"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B116" s="1"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B124" s="1"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B125" s="1"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B126" s="1"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B127" s="1"/>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B128" s="1"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B129" s="1"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B130" s="1"/>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B131" s="1"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B132" s="1"/>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B133" s="1"/>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B134" s="1"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B135" s="1"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B136" s="1"/>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B137" s="1"/>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B138" s="1"/>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B139" s="1"/>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B140" s="1"/>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B141" s="1"/>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B142" s="1"/>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B143" s="1"/>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B144" s="1"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B145" s="1"/>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B146" s="1"/>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B147" s="1"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B148" s="1"/>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B149" s="1"/>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B150" s="1"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B151" s="1"/>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B152" s="1"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B153" s="1"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B154" s="1"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B155" s="1"/>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B156" s="1"/>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B157" s="1"/>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B158" s="1"/>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B159" s="1"/>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B160" s="1"/>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B161" s="1"/>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B162" s="1"/>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B163" s="1"/>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B164" s="1"/>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B165" s="1"/>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B166" s="1"/>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B167" s="1"/>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B168" s="1"/>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B169" s="1"/>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B170" s="1"/>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B171" s="1"/>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B172" s="1"/>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B173" s="1"/>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B174" s="1"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B175" s="1"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B176" s="1"/>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B177" s="1"/>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B178" s="1"/>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B179" s="1"/>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B180" s="1"/>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B181" s="1"/>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B182" s="1"/>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B183" s="1"/>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B184" s="1"/>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B185" s="1"/>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B186" s="1"/>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B187" s="1"/>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B188" s="1"/>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B189" s="1"/>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B190" s="1"/>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B191" s="1"/>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B192" s="1"/>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B193" s="1"/>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B194" s="1"/>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B195" s="1"/>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B196" s="1"/>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B197" s="1"/>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B198" s="1"/>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B199" s="1"/>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B200" s="1"/>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B201" s="1"/>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B202" s="1"/>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B203" s="1"/>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B204" s="1"/>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B205" s="1"/>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B206" s="1"/>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B207" s="1"/>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B208" s="1"/>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B209" s="1"/>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B210" s="1"/>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B211" s="1"/>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B212" s="1"/>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B213" s="1"/>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B214" s="1"/>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B215" s="1"/>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B216" s="1"/>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B217" s="1"/>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B218" s="1"/>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B219" s="1"/>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B220" s="1"/>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B221" s="1"/>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B222" s="1"/>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B223" s="1"/>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B224" s="1"/>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B225" s="1"/>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B226" s="1"/>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B227" s="1"/>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B228" s="1"/>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B229" s="1"/>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B230" s="1"/>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B231" s="1"/>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B232" s="1"/>
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B233" s="1"/>
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B234" s="1"/>
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B235" s="1"/>
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B236" s="1"/>
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B237" s="1"/>
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B238" s="1"/>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B239" s="1"/>
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B240" s="1"/>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B241" s="1"/>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B242" s="1"/>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B243" s="1"/>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B244" s="1"/>
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B245" s="1"/>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B246" s="1"/>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B247" s="1"/>
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B248" s="1"/>
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B249" s="1"/>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B250" s="1"/>
+    </row>
+    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B251" s="1"/>
+    </row>
+    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B252" s="1"/>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B253" s="1"/>
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B254" s="1"/>
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B255" s="1"/>
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B256" s="1"/>
+    </row>
+    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B257" s="1"/>
+    </row>
+    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B258" s="1"/>
+    </row>
+    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B259" s="1"/>
+    </row>
+    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B260" s="1"/>
+    </row>
+    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B261" s="1"/>
+    </row>
+    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B262" s="1"/>
+    </row>
+    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B263" s="1"/>
+    </row>
+    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B264" s="1"/>
+    </row>
+    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B265" s="1"/>
+    </row>
+    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B266" s="1"/>
+    </row>
+    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B267" s="1"/>
+    </row>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B268" s="1"/>
+    </row>
+    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B269" s="1"/>
+    </row>
+    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B270" s="1"/>
+    </row>
+    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B271" s="1"/>
+    </row>
+    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B272" s="1"/>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B273" s="1"/>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B274" s="1"/>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B275" s="1"/>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B276" s="1"/>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B277" s="1"/>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B278" s="1"/>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B279" s="1"/>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B280" s="1"/>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B281" s="1"/>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B282" s="1"/>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B283" s="1"/>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B284" s="1"/>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B285" s="1"/>
+    </row>
+    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B286" s="1"/>
+    </row>
+    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B287" s="1"/>
+    </row>
+    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B288" s="1"/>
+    </row>
+    <row r="289" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B289" s="1"/>
+    </row>
+    <row r="290" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B290" s="1"/>
+    </row>
+    <row r="291" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B291" s="1"/>
+    </row>
+    <row r="292" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B292" s="1"/>
+    </row>
+    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B293" s="1"/>
+    </row>
+    <row r="294" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B294" s="1"/>
+    </row>
+    <row r="295" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B295" s="1"/>
+    </row>
+    <row r="296" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B296" s="1"/>
+    </row>
+    <row r="297" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B297" s="1"/>
+    </row>
+    <row r="298" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B298" s="1"/>
+    </row>
+    <row r="299" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B299" s="1"/>
+    </row>
+    <row r="300" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B300" s="1"/>
+    </row>
+    <row r="301" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B301" s="1"/>
+    </row>
+    <row r="302" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B302" s="1"/>
+    </row>
+    <row r="303" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B303" s="1"/>
+    </row>
+    <row r="304" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B304" s="1"/>
+    </row>
+    <row r="305" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B305" s="1"/>
+    </row>
+    <row r="306" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B306" s="1"/>
+    </row>
+    <row r="307" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B307" s="1"/>
+    </row>
+    <row r="308" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B308" s="1"/>
+    </row>
+    <row r="309" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B309" s="1"/>
+    </row>
+    <row r="310" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B310" s="1"/>
+    </row>
+    <row r="311" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B311" s="1"/>
+    </row>
+    <row r="312" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B312" s="1"/>
+    </row>
+    <row r="313" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B313" s="1"/>
+    </row>
+    <row r="314" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B314" s="1"/>
+    </row>
+    <row r="315" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B315" s="1"/>
+    </row>
+    <row r="316" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B316" s="1"/>
+    </row>
+    <row r="317" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B317" s="1"/>
+    </row>
+    <row r="318" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B318" s="1"/>
+    </row>
+    <row r="319" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B319" s="1"/>
+    </row>
+    <row r="320" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B320" s="1"/>
+    </row>
+    <row r="321" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B321" s="1"/>
+    </row>
+    <row r="322" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B322" s="1"/>
+    </row>
+    <row r="323" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B323" s="1"/>
+    </row>
+    <row r="324" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B324" s="1"/>
+    </row>
+    <row r="325" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B325" s="1"/>
+    </row>
+    <row r="326" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B326" s="1"/>
+    </row>
+    <row r="327" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B327" s="1"/>
+    </row>
+    <row r="328" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B328" s="1"/>
+    </row>
+    <row r="329" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B329" s="1"/>
+    </row>
+    <row r="330" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B330" s="1"/>
+    </row>
+    <row r="331" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B331" s="1"/>
+    </row>
+    <row r="332" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B332" s="1"/>
+    </row>
+    <row r="333" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B333" s="1"/>
+    </row>
+    <row r="334" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B334" s="1"/>
+    </row>
+    <row r="335" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B335" s="1"/>
+    </row>
+    <row r="336" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B336" s="1"/>
+    </row>
+    <row r="337" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B337" s="1"/>
+    </row>
+    <row r="338" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B338" s="1"/>
+    </row>
+    <row r="339" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B339" s="1"/>
+    </row>
+    <row r="340" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B340" s="1"/>
+    </row>
+    <row r="341" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B341" s="1"/>
+    </row>
+    <row r="342" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B342" s="1"/>
+    </row>
+    <row r="343" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B343" s="1"/>
+    </row>
+    <row r="344" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B344" s="1"/>
+    </row>
+    <row r="345" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B345" s="1"/>
+    </row>
+    <row r="346" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B346" s="1"/>
+    </row>
+    <row r="347" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B347" s="1"/>
+    </row>
+    <row r="348" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B348" s="1"/>
+    </row>
+    <row r="349" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B349" s="1"/>
+    </row>
+    <row r="350" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B350" s="1"/>
+    </row>
+    <row r="351" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B351" s="1"/>
+    </row>
+    <row r="352" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B352" s="1"/>
+    </row>
+    <row r="353" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B353" s="1"/>
+    </row>
+    <row r="354" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B354" s="1"/>
+    </row>
+    <row r="355" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B355" s="1"/>
+    </row>
+    <row r="356" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B356" s="1"/>
+    </row>
+    <row r="357" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B357" s="1"/>
+    </row>
+    <row r="358" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B358" s="1"/>
+    </row>
+    <row r="359" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B359" s="1"/>
+    </row>
+    <row r="360" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B360" s="1"/>
+    </row>
+    <row r="361" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B361" s="1"/>
+    </row>
+    <row r="362" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B362" s="1"/>
+    </row>
+    <row r="363" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B363" s="1"/>
+    </row>
+    <row r="364" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B364" s="1"/>
+    </row>
+    <row r="365" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B365" s="1"/>
+    </row>
+    <row r="366" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B366" s="1"/>
+    </row>
+    <row r="367" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B367" s="1"/>
+    </row>
+    <row r="368" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B368" s="1"/>
+    </row>
+    <row r="369" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B369" s="1"/>
+    </row>
+    <row r="370" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B370" s="1"/>
+    </row>
+    <row r="371" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B371" s="1"/>
+    </row>
+    <row r="372" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B372" s="1"/>
+    </row>
+    <row r="373" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B373" s="1"/>
+    </row>
+    <row r="374" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B374" s="1"/>
+    </row>
+    <row r="375" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B375" s="1"/>
+    </row>
+    <row r="376" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B376" s="1"/>
+    </row>
+    <row r="377" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B377" s="1"/>
+    </row>
+    <row r="378" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B378" s="1"/>
+    </row>
+    <row r="379" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B379" s="1"/>
+    </row>
+    <row r="380" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B380" s="1"/>
+    </row>
+    <row r="381" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B381" s="1"/>
+    </row>
+    <row r="382" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B382" s="1"/>
+    </row>
+    <row r="383" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B383" s="1"/>
+    </row>
+    <row r="384" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B384" s="1"/>
+    </row>
+    <row r="385" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B385" s="1"/>
+    </row>
+    <row r="386" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B386" s="1"/>
+    </row>
+    <row r="387" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B387" s="1"/>
+    </row>
+    <row r="388" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B388" s="1"/>
+    </row>
+    <row r="389" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B389" s="1"/>
+    </row>
+    <row r="390" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B390" s="1"/>
+    </row>
+    <row r="391" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B391" s="1"/>
+    </row>
+    <row r="392" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B392" s="1"/>
+    </row>
+    <row r="393" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B393" s="1"/>
+    </row>
+    <row r="394" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B394" s="1"/>
+    </row>
+    <row r="395" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B395" s="1"/>
+    </row>
+    <row r="396" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B396" s="1"/>
+    </row>
+    <row r="397" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B397" s="1"/>
+    </row>
+    <row r="398" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B398" s="1"/>
+    </row>
+    <row r="399" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B399" s="1"/>
+    </row>
+    <row r="400" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B400" s="1"/>
+    </row>
+    <row r="401" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B401" s="1"/>
+    </row>
+    <row r="402" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B402" s="1"/>
+    </row>
+    <row r="403" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B403" s="1"/>
+    </row>
+    <row r="404" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B404" s="1"/>
+    </row>
+    <row r="405" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B405" s="1"/>
+    </row>
+    <row r="406" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B406" s="1"/>
+    </row>
+    <row r="407" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B407" s="1"/>
+    </row>
+    <row r="408" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B408" s="1"/>
+    </row>
+    <row r="409" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B409" s="1"/>
+    </row>
+    <row r="410" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B410" s="1"/>
+    </row>
+    <row r="411" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B411" s="1"/>
+    </row>
+    <row r="412" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B412" s="1"/>
+    </row>
+    <row r="413" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B413" s="1"/>
+    </row>
+    <row r="414" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B414" s="1"/>
+    </row>
+    <row r="415" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B415" s="1"/>
+    </row>
+    <row r="416" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B416" s="1"/>
+    </row>
+    <row r="417" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B417" s="1"/>
+    </row>
+    <row r="418" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B418" s="1"/>
+    </row>
+    <row r="419" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B419" s="1"/>
+    </row>
+    <row r="420" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B420" s="1"/>
+    </row>
+    <row r="421" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B421" s="1"/>
+    </row>
+    <row r="422" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B422" s="1"/>
+    </row>
+    <row r="423" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B423" s="1"/>
+    </row>
+    <row r="424" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B424" s="1"/>
+    </row>
+    <row r="425" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B425" s="1"/>
+    </row>
+    <row r="426" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B426" s="1"/>
+    </row>
+    <row r="427" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B427" s="1"/>
+    </row>
+    <row r="428" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B428" s="1"/>
+    </row>
+    <row r="429" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B429" s="1"/>
+    </row>
+    <row r="430" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B430" s="1"/>
+    </row>
+    <row r="431" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B431" s="1"/>
+    </row>
+    <row r="432" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B432" s="1"/>
+    </row>
+    <row r="433" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B433" s="1"/>
+    </row>
+    <row r="434" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B434" s="1"/>
+    </row>
+    <row r="435" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B435" s="1"/>
+    </row>
+    <row r="436" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B436" s="1"/>
+    </row>
+    <row r="437" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B437" s="1"/>
+    </row>
+    <row r="438" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B438" s="1"/>
+    </row>
+    <row r="439" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B439" s="1"/>
+    </row>
+    <row r="440" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B440" s="1"/>
+    </row>
+    <row r="441" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B441" s="1"/>
+    </row>
+    <row r="442" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B442" s="1"/>
+    </row>
+    <row r="443" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B443" s="1"/>
+    </row>
+    <row r="444" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B444" s="1"/>
+    </row>
+    <row r="445" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B445" s="1"/>
+    </row>
+    <row r="446" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B446" s="1"/>
+    </row>
+    <row r="447" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B447" s="1"/>
+    </row>
+    <row r="448" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B448" s="1"/>
+    </row>
+    <row r="449" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B449" s="1"/>
+    </row>
+    <row r="450" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B450" s="1"/>
+    </row>
+    <row r="451" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B451" s="1"/>
+    </row>
+    <row r="452" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B452" s="1"/>
+    </row>
+    <row r="453" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B453" s="1"/>
+    </row>
+    <row r="454" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B454" s="1"/>
+    </row>
+    <row r="455" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B455" s="1"/>
+    </row>
+    <row r="456" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B456" s="1"/>
+    </row>
+    <row r="457" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B457" s="1"/>
+    </row>
+    <row r="458" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B458" s="1"/>
+    </row>
+    <row r="459" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B459" s="1"/>
+    </row>
+    <row r="460" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B460" s="1"/>
+    </row>
+    <row r="461" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B461" s="1"/>
+    </row>
+    <row r="462" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B462" s="1"/>
+    </row>
+    <row r="463" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B463" s="1"/>
+    </row>
+    <row r="464" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B464" s="1"/>
+    </row>
+    <row r="465" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B465" s="1"/>
+    </row>
+    <row r="466" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B466" s="1"/>
+    </row>
+    <row r="467" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B467" s="1"/>
+    </row>
+    <row r="468" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B468" s="1"/>
+    </row>
+    <row r="469" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B469" s="1"/>
+    </row>
+    <row r="470" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B470" s="1"/>
+    </row>
+    <row r="471" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B471" s="1"/>
+    </row>
+    <row r="472" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B472" s="1"/>
+    </row>
+    <row r="473" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B473" s="1"/>
+    </row>
+    <row r="474" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B474" s="1"/>
+    </row>
+    <row r="475" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B475" s="1"/>
+    </row>
+    <row r="476" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B476" s="1"/>
+    </row>
+    <row r="477" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B477" s="1"/>
+    </row>
+    <row r="478" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B478" s="1"/>
+    </row>
+    <row r="479" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B479" s="1"/>
+    </row>
+    <row r="480" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B480" s="1"/>
+    </row>
+    <row r="481" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B481" s="1"/>
+    </row>
+    <row r="482" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B482" s="1"/>
+    </row>
+    <row r="483" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B483" s="1"/>
+    </row>
+    <row r="484" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B484" s="1"/>
+    </row>
+    <row r="485" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B485" s="1"/>
+    </row>
+    <row r="486" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B486" s="1"/>
+    </row>
+    <row r="487" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B487" s="1"/>
+    </row>
+    <row r="488" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B488" s="1"/>
+    </row>
+    <row r="489" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B489" s="1"/>
+    </row>
+    <row r="490" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B490" s="1"/>
+    </row>
+    <row r="491" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B491" s="1"/>
+    </row>
+    <row r="492" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B492" s="1"/>
+    </row>
+    <row r="493" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B493" s="1"/>
+    </row>
+    <row r="494" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B494" s="1"/>
+    </row>
+    <row r="495" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B495" s="1"/>
+    </row>
+    <row r="496" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B496" s="1"/>
+    </row>
+    <row r="497" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B497" s="1"/>
+    </row>
+    <row r="498" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B498" s="1"/>
+    </row>
+    <row r="499" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B499" s="1"/>
+    </row>
+    <row r="500" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B500" s="1"/>
+    </row>
+    <row r="501" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B501" s="1"/>
+    </row>
+    <row r="502" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B502" s="1"/>
+    </row>
+    <row r="503" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B503" s="1"/>
+    </row>
+    <row r="504" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B504" s="1"/>
+    </row>
+    <row r="505" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B505" s="1"/>
+    </row>
+    <row r="506" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B506" s="1"/>
+    </row>
+    <row r="507" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B507" s="1"/>
+    </row>
+    <row r="508" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B508" s="1"/>
+    </row>
+    <row r="509" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B509" s="1"/>
+    </row>
+    <row r="510" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B510" s="1"/>
+    </row>
+    <row r="511" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B511" s="1"/>
+    </row>
+    <row r="512" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B512" s="1"/>
+    </row>
+    <row r="513" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B513" s="1"/>
+    </row>
+    <row r="514" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B514" s="1"/>
+    </row>
+    <row r="515" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B515" s="1"/>
+    </row>
+    <row r="516" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B516" s="1"/>
+    </row>
+    <row r="517" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B517" s="1"/>
+    </row>
+    <row r="518" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B518" s="1"/>
+    </row>
+    <row r="519" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B519" s="1"/>
+    </row>
+    <row r="520" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B520" s="1"/>
+    </row>
+    <row r="521" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B521" s="1"/>
+    </row>
+    <row r="522" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B522" s="1"/>
+    </row>
+    <row r="523" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B523" s="1"/>
+    </row>
+    <row r="524" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B524" s="1"/>
+    </row>
+    <row r="525" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B525" s="1"/>
+    </row>
+    <row r="526" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B526" s="1"/>
+    </row>
+    <row r="527" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B527" s="1"/>
+    </row>
+    <row r="528" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B528" s="1"/>
+    </row>
+    <row r="529" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B529" s="1"/>
+    </row>
+    <row r="530" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B530" s="1"/>
+    </row>
+    <row r="531" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B531" s="1"/>
+    </row>
+    <row r="532" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B532" s="1"/>
+    </row>
+    <row r="533" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B533" s="1"/>
+    </row>
+    <row r="534" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B534" s="1"/>
+    </row>
+    <row r="535" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B535" s="1"/>
+    </row>
+    <row r="536" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B536" s="1"/>
+    </row>
+    <row r="537" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B537" s="1"/>
+    </row>
+    <row r="538" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B538" s="1"/>
+    </row>
+    <row r="539" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B539" s="1"/>
+    </row>
+    <row r="540" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B540" s="1"/>
+    </row>
+    <row r="541" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B541" s="1"/>
+    </row>
+    <row r="542" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B542" s="1"/>
+    </row>
+    <row r="543" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B543" s="1"/>
+    </row>
+    <row r="544" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B544" s="1"/>
+    </row>
+    <row r="545" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B545" s="1"/>
+    </row>
+    <row r="546" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B546" s="1"/>
+    </row>
+    <row r="547" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B547" s="1"/>
+    </row>
+    <row r="548" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B548" s="1"/>
+    </row>
+    <row r="549" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B549" s="1"/>
+    </row>
+    <row r="550" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B550" s="1"/>
+    </row>
+    <row r="551" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B551" s="1"/>
+    </row>
+    <row r="552" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B552" s="1"/>
+    </row>
+    <row r="553" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B553" s="1"/>
+    </row>
+    <row r="554" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B554" s="1"/>
+    </row>
+    <row r="555" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B555" s="1"/>
+    </row>
+    <row r="556" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B556" s="1"/>
+    </row>
+    <row r="557" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B557" s="1"/>
+    </row>
+    <row r="558" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B558" s="1"/>
+    </row>
+    <row r="559" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B559" s="1"/>
+    </row>
+    <row r="560" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B560" s="1"/>
+    </row>
+    <row r="561" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B561" s="1"/>
+    </row>
+    <row r="562" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B562" s="1"/>
+    </row>
+    <row r="563" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B563" s="1"/>
+    </row>
+    <row r="564" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B564" s="1"/>
+    </row>
+    <row r="565" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B565" s="1"/>
+    </row>
+    <row r="566" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B566" s="1"/>
+    </row>
+    <row r="567" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B567" s="1"/>
+    </row>
+    <row r="568" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B568" s="1"/>
+    </row>
+    <row r="569" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B569" s="1"/>
+    </row>
+    <row r="570" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B570" s="1"/>
+    </row>
+    <row r="571" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B571" s="1"/>
+    </row>
+    <row r="572" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B572" s="1"/>
+    </row>
+    <row r="573" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B573" s="1"/>
+    </row>
+    <row r="574" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B574" s="1"/>
+    </row>
+    <row r="575" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B575" s="1"/>
+    </row>
+    <row r="576" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B576" s="1"/>
+    </row>
+    <row r="577" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B577" s="1"/>
+    </row>
+    <row r="578" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B578" s="1"/>
+    </row>
+    <row r="579" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B579" s="1"/>
+    </row>
+    <row r="580" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B580" s="1"/>
+    </row>
+    <row r="581" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B581" s="1"/>
+    </row>
+    <row r="582" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B582" s="1"/>
+    </row>
+    <row r="583" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B583" s="1"/>
+    </row>
+    <row r="584" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B584" s="1"/>
+    </row>
+    <row r="585" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B585" s="1"/>
+    </row>
+    <row r="586" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B586" s="1"/>
+    </row>
+    <row r="587" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B587" s="1"/>
+    </row>
+    <row r="588" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B588" s="1"/>
+    </row>
+    <row r="589" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B589" s="1"/>
+    </row>
+    <row r="590" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B590" s="1"/>
+    </row>
+    <row r="591" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B591" s="1"/>
+    </row>
+    <row r="592" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B592" s="1"/>
+    </row>
+    <row r="593" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B593" s="1"/>
+    </row>
+    <row r="594" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B594" s="1"/>
+    </row>
+    <row r="595" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B595" s="1"/>
+    </row>
+    <row r="596" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B596" s="1"/>
+    </row>
+    <row r="597" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B597" s="1"/>
+    </row>
+    <row r="598" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B598" s="1"/>
+    </row>
+    <row r="599" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B599" s="1"/>
+    </row>
+    <row r="600" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B600" s="1"/>
+    </row>
+    <row r="601" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B601" s="1"/>
+    </row>
+    <row r="602" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B602" s="1"/>
+    </row>
+    <row r="603" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B603" s="1"/>
+    </row>
+    <row r="604" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B604" s="1"/>
+    </row>
+    <row r="605" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B605" s="1"/>
+    </row>
+    <row r="606" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B606" s="1"/>
+    </row>
+    <row r="607" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B607" s="1"/>
+    </row>
+    <row r="608" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B608" s="1"/>
+    </row>
+    <row r="609" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B609" s="1"/>
+    </row>
+    <row r="610" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B610" s="1"/>
+    </row>
+    <row r="611" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B611" s="1"/>
+    </row>
+    <row r="612" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B612" s="1"/>
+    </row>
+    <row r="613" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B613" s="1"/>
+    </row>
+    <row r="614" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B614" s="1"/>
+    </row>
+    <row r="615" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B615" s="1"/>
+    </row>
+    <row r="616" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B616" s="1"/>
+    </row>
+    <row r="617" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B617" s="1"/>
+    </row>
+    <row r="618" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B618" s="1"/>
+    </row>
+    <row r="619" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B619" s="1"/>
+    </row>
+    <row r="620" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B620" s="1"/>
+    </row>
+    <row r="621" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B621" s="1"/>
+    </row>
+    <row r="622" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B622" s="1"/>
+    </row>
+    <row r="623" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B623" s="1"/>
+    </row>
+    <row r="624" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B624" s="1"/>
+    </row>
+    <row r="625" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B625" s="1"/>
+    </row>
+    <row r="626" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B626" s="1"/>
+    </row>
+    <row r="627" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B627" s="1"/>
+    </row>
+    <row r="628" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B628" s="1"/>
+    </row>
+    <row r="629" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B629" s="1"/>
+    </row>
+    <row r="630" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B630" s="1"/>
+    </row>
+    <row r="631" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B631" s="1"/>
+    </row>
+    <row r="632" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B632" s="1"/>
+    </row>
+    <row r="633" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B633" s="1"/>
+    </row>
+    <row r="634" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B634" s="1"/>
+    </row>
+    <row r="635" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B635" s="1"/>
+    </row>
+    <row r="636" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B636" s="1"/>
+    </row>
+    <row r="637" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B637" s="1"/>
+    </row>
+    <row r="638" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B638" s="1"/>
+    </row>
+    <row r="639" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B639" s="1"/>
+    </row>
+    <row r="640" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B640" s="1"/>
+    </row>
+    <row r="641" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B641" s="1"/>
+    </row>
+    <row r="642" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B642" s="1"/>
+    </row>
+    <row r="643" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B643" s="1"/>
+    </row>
+    <row r="644" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B644" s="1"/>
+    </row>
+    <row r="645" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B645" s="1"/>
+    </row>
+    <row r="646" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B646" s="1"/>
+    </row>
+    <row r="647" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B647" s="1"/>
+    </row>
+    <row r="648" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B648" s="1"/>
+    </row>
+    <row r="649" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B649" s="1"/>
+    </row>
+    <row r="650" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B650" s="1"/>
+    </row>
+    <row r="651" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B651" s="1"/>
+    </row>
+    <row r="652" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B652" s="1"/>
+    </row>
+    <row r="653" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B653" s="1"/>
+    </row>
+    <row r="654" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B654" s="1"/>
+    </row>
+    <row r="655" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B655" s="1"/>
+    </row>
+    <row r="656" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B656" s="1"/>
+    </row>
+    <row r="657" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B657" s="1"/>
+    </row>
+    <row r="658" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B658" s="1"/>
+    </row>
+    <row r="659" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B659" s="1"/>
+    </row>
+    <row r="660" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B660" s="1"/>
+    </row>
+    <row r="661" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B661" s="1"/>
+    </row>
+    <row r="662" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B662" s="1"/>
+    </row>
+    <row r="663" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B663" s="1"/>
+    </row>
+    <row r="664" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B664" s="1"/>
+    </row>
+    <row r="665" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B665" s="1"/>
+    </row>
+    <row r="666" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B666" s="1"/>
+    </row>
+    <row r="667" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B667" s="1"/>
+    </row>
+    <row r="668" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B668" s="1"/>
+    </row>
+    <row r="669" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B669" s="1"/>
+    </row>
+    <row r="670" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B670" s="1"/>
+    </row>
+    <row r="671" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B671" s="1"/>
+    </row>
+    <row r="672" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B672" s="1"/>
+    </row>
+    <row r="673" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B673" s="1"/>
+    </row>
+    <row r="674" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B674" s="1"/>
+    </row>
+    <row r="675" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B675" s="1"/>
+    </row>
+    <row r="676" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B676" s="1"/>
+    </row>
+    <row r="677" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B677" s="1"/>
+    </row>
+    <row r="678" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B678" s="1"/>
+    </row>
+    <row r="679" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B679" s="1"/>
+    </row>
+    <row r="680" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B680" s="1"/>
+    </row>
+    <row r="681" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B681" s="1"/>
+    </row>
+    <row r="682" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B682" s="1"/>
+    </row>
+    <row r="683" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B683" s="1"/>
+    </row>
+    <row r="684" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B684" s="1"/>
+    </row>
+    <row r="685" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B685" s="1"/>
+    </row>
+    <row r="686" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B686" s="1"/>
+    </row>
+    <row r="687" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B687" s="1"/>
+    </row>
+    <row r="688" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B688" s="1"/>
+    </row>
+    <row r="689" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B689" s="1"/>
+    </row>
+    <row r="690" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B690" s="1"/>
+    </row>
+    <row r="691" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B691" s="1"/>
+    </row>
+    <row r="692" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B692" s="1"/>
+    </row>
+    <row r="693" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B693" s="1"/>
+    </row>
+    <row r="694" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B694" s="1"/>
+    </row>
+    <row r="695" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B695" s="1"/>
+    </row>
+    <row r="696" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B696" s="1"/>
+    </row>
+    <row r="697" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B697" s="1"/>
+    </row>
+    <row r="698" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B698" s="1"/>
+    </row>
+    <row r="699" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B699" s="1"/>
+    </row>
+    <row r="700" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B700" s="1"/>
+    </row>
+    <row r="701" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B701" s="1"/>
+    </row>
+    <row r="702" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B702" s="1"/>
+    </row>
+    <row r="703" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B703" s="1"/>
+    </row>
+    <row r="704" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B704" s="1"/>
+    </row>
+    <row r="705" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B705" s="1"/>
+    </row>
+    <row r="706" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B706" s="1"/>
+    </row>
+    <row r="707" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B707" s="1"/>
+    </row>
+    <row r="708" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B708" s="1"/>
+    </row>
+    <row r="709" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B709" s="1"/>
+    </row>
+    <row r="710" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B710" s="1"/>
+    </row>
+    <row r="711" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B711" s="1"/>
+    </row>
+    <row r="712" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B712" s="1"/>
+    </row>
+    <row r="713" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B713" s="1"/>
+    </row>
+    <row r="714" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B714" s="1"/>
+    </row>
+    <row r="715" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B715" s="1"/>
+    </row>
+    <row r="716" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B716" s="1"/>
+    </row>
+    <row r="717" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B717" s="1"/>
+    </row>
+    <row r="718" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B718" s="1"/>
+    </row>
+    <row r="719" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B719" s="1"/>
+    </row>
+    <row r="720" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B720" s="1"/>
+    </row>
+    <row r="721" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B721" s="1"/>
+    </row>
+    <row r="722" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B722" s="1"/>
+    </row>
+    <row r="723" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B723" s="1"/>
+    </row>
+    <row r="724" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B724" s="1"/>
+    </row>
+    <row r="725" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B725" s="1"/>
+    </row>
+    <row r="726" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B726" s="1"/>
+    </row>
+    <row r="727" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B727" s="1"/>
+    </row>
+    <row r="728" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B728" s="1"/>
+    </row>
+    <row r="729" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B729" s="1"/>
+    </row>
+    <row r="730" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B730" s="1"/>
+    </row>
+    <row r="731" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B731" s="1"/>
+    </row>
+    <row r="732" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B732" s="1"/>
+    </row>
+    <row r="733" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B733" s="1"/>
+    </row>
+    <row r="734" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B734" s="1"/>
+    </row>
+    <row r="735" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B735" s="1"/>
+    </row>
+    <row r="736" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B736" s="1"/>
+    </row>
+    <row r="737" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B737" s="1"/>
+    </row>
+    <row r="738" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B738" s="1"/>
+    </row>
+    <row r="739" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B739" s="1"/>
+    </row>
+    <row r="740" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B740" s="1"/>
+    </row>
+    <row r="741" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B741" s="1"/>
+    </row>
+    <row r="742" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B742" s="1"/>
+    </row>
+    <row r="743" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B743" s="1"/>
+    </row>
+    <row r="744" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B744" s="1"/>
+    </row>
+    <row r="745" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B745" s="1"/>
+    </row>
+    <row r="746" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B746" s="1"/>
+    </row>
+    <row r="747" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B747" s="1"/>
+    </row>
+    <row r="748" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B748" s="1"/>
+    </row>
+    <row r="749" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B749" s="1"/>
+    </row>
+    <row r="750" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B750" s="1"/>
+    </row>
+    <row r="751" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B751" s="1"/>
+    </row>
+    <row r="752" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B752" s="1"/>
+    </row>
+    <row r="753" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B753" s="1"/>
+    </row>
+    <row r="754" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B754" s="1"/>
+    </row>
+    <row r="755" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B755" s="1"/>
+    </row>
+    <row r="756" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B756" s="1"/>
+    </row>
+    <row r="757" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B757" s="1"/>
+    </row>
+    <row r="758" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B758" s="1"/>
+    </row>
+    <row r="759" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B759" s="1"/>
+    </row>
+    <row r="760" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B760" s="1"/>
+    </row>
+    <row r="761" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B761" s="1"/>
+    </row>
+    <row r="762" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B762" s="1"/>
+    </row>
+    <row r="763" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B763" s="1"/>
+    </row>
+    <row r="764" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B764" s="1"/>
+    </row>
+    <row r="765" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B765" s="1"/>
+    </row>
+    <row r="766" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B766" s="1"/>
+    </row>
+    <row r="767" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B767" s="1"/>
+    </row>
+    <row r="768" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B768" s="1"/>
+    </row>
+    <row r="769" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B769" s="1"/>
+    </row>
+    <row r="770" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B770" s="1"/>
+    </row>
+    <row r="771" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B771" s="1"/>
+    </row>
+    <row r="772" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B772" s="1"/>
+    </row>
+    <row r="773" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B773" s="1"/>
+    </row>
+    <row r="774" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B774" s="1"/>
+    </row>
+    <row r="775" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B775" s="1"/>
+    </row>
+    <row r="776" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B776" s="1"/>
+    </row>
+    <row r="777" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B777" s="1"/>
+    </row>
+    <row r="778" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B778" s="1"/>
+    </row>
+    <row r="779" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B779" s="1"/>
+    </row>
+    <row r="780" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B780" s="1"/>
+    </row>
+    <row r="781" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B781" s="1"/>
+    </row>
+    <row r="782" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B782" s="1"/>
+    </row>
+    <row r="783" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B783" s="1"/>
+    </row>
+    <row r="784" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B784" s="1"/>
+    </row>
+    <row r="785" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B785" s="1"/>
+    </row>
+    <row r="786" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B786" s="1"/>
+    </row>
+    <row r="787" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B787" s="1"/>
+    </row>
+    <row r="788" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B788" s="1"/>
+    </row>
+    <row r="789" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B789" s="1"/>
+    </row>
+    <row r="790" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B790" s="1"/>
+    </row>
+    <row r="791" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B791" s="1"/>
+    </row>
+    <row r="792" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B792" s="1"/>
+    </row>
+    <row r="793" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B793" s="1"/>
+    </row>
+    <row r="794" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B794" s="1"/>
+    </row>
+    <row r="795" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B795" s="1"/>
+    </row>
+    <row r="796" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B796" s="1"/>
+    </row>
+    <row r="797" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B797" s="1"/>
+    </row>
+    <row r="798" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B798" s="1"/>
+    </row>
+    <row r="799" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B799" s="1"/>
+    </row>
+    <row r="800" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B800" s="1"/>
+    </row>
+    <row r="801" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B801" s="1"/>
+    </row>
+    <row r="802" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B802" s="1"/>
+    </row>
+    <row r="803" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B803" s="1"/>
+    </row>
+    <row r="804" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B804" s="1"/>
+    </row>
+    <row r="805" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B805" s="1"/>
+    </row>
+    <row r="806" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B806" s="1"/>
+    </row>
+    <row r="807" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B807" s="1"/>
+    </row>
+    <row r="808" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B808" s="1"/>
+    </row>
+    <row r="809" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B809" s="1"/>
+    </row>
+    <row r="810" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B810" s="1"/>
+    </row>
+    <row r="811" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B811" s="1"/>
+    </row>
+    <row r="812" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B812" s="1"/>
+    </row>
+    <row r="813" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B813" s="1"/>
+    </row>
+    <row r="814" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B814" s="1"/>
+    </row>
+    <row r="815" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B815" s="1"/>
+    </row>
+    <row r="816" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B816" s="1"/>
+    </row>
+    <row r="817" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B817" s="1"/>
+    </row>
+    <row r="818" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B818" s="1"/>
+    </row>
+    <row r="819" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B819" s="1"/>
+    </row>
+    <row r="820" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B820" s="1"/>
+    </row>
+    <row r="821" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B821" s="1"/>
+    </row>
+    <row r="822" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B822" s="1"/>
+    </row>
+    <row r="823" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B823" s="1"/>
+    </row>
+    <row r="824" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B824" s="1"/>
+    </row>
+    <row r="825" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B825" s="1"/>
+    </row>
+    <row r="826" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B826" s="1"/>
+    </row>
+    <row r="827" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B827" s="1"/>
+    </row>
+    <row r="828" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B828" s="1"/>
+    </row>
+    <row r="829" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B829" s="1"/>
+    </row>
+    <row r="830" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B830" s="1"/>
+    </row>
+    <row r="831" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B831" s="1"/>
+    </row>
+    <row r="832" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B832" s="1"/>
+    </row>
+    <row r="833" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B833" s="1"/>
+    </row>
+    <row r="834" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B834" s="1"/>
+    </row>
+    <row r="835" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B835" s="1"/>
+    </row>
+    <row r="836" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B836" s="1"/>
+    </row>
+    <row r="837" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B837" s="1"/>
+    </row>
+    <row r="838" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B838" s="1"/>
+    </row>
+    <row r="839" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B839" s="1"/>
+    </row>
+    <row r="840" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B840" s="1"/>
+    </row>
+    <row r="841" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B841" s="1"/>
+    </row>
+    <row r="842" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B842" s="1"/>
+    </row>
+    <row r="843" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B843" s="1"/>
+    </row>
+    <row r="844" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B844" s="1"/>
+    </row>
+    <row r="845" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B845" s="1"/>
+    </row>
+    <row r="846" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B846" s="1"/>
+    </row>
+    <row r="847" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B847" s="1"/>
+    </row>
+    <row r="848" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B848" s="1"/>
+    </row>
+    <row r="849" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B849" s="1"/>
+    </row>
+    <row r="850" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B850" s="1"/>
+    </row>
+    <row r="851" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B851" s="1"/>
+    </row>
+    <row r="852" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B852" s="1"/>
+    </row>
+    <row r="853" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B853" s="1"/>
+    </row>
+    <row r="854" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B854" s="1"/>
+    </row>
+    <row r="855" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B855" s="1"/>
+    </row>
+    <row r="856" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B856" s="1"/>
+    </row>
+    <row r="857" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B857" s="1"/>
+    </row>
+    <row r="858" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B858" s="1"/>
+    </row>
+    <row r="859" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B859" s="1"/>
+    </row>
+    <row r="860" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B860" s="1"/>
+    </row>
+    <row r="861" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B861" s="1"/>
+    </row>
+    <row r="862" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B862" s="1"/>
+    </row>
+    <row r="863" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B863" s="1"/>
+    </row>
+    <row r="864" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B864" s="1"/>
+    </row>
+    <row r="865" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B865" s="1"/>
+    </row>
+    <row r="866" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B866" s="1"/>
+    </row>
+    <row r="867" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B867" s="1"/>
+    </row>
+    <row r="868" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B868" s="1"/>
+    </row>
+    <row r="869" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B869" s="1"/>
+    </row>
+    <row r="870" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B870" s="1"/>
+    </row>
+    <row r="871" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B871" s="1"/>
+    </row>
+    <row r="872" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B872" s="1"/>
+    </row>
+    <row r="873" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B873" s="1"/>
+    </row>
+    <row r="874" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B874" s="1"/>
+    </row>
+    <row r="875" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B875" s="1"/>
+    </row>
+    <row r="876" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B876" s="1"/>
+    </row>
+    <row r="877" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B877" s="1"/>
+    </row>
+    <row r="878" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B878" s="1"/>
+    </row>
+    <row r="879" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B879" s="1"/>
+    </row>
+    <row r="880" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B880" s="1"/>
+    </row>
+    <row r="881" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B881" s="1"/>
+    </row>
+    <row r="882" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B882" s="1"/>
+    </row>
+    <row r="883" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B883" s="1"/>
+    </row>
+    <row r="884" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B884" s="1"/>
+    </row>
+    <row r="885" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B885" s="1"/>
+    </row>
+    <row r="886" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B886" s="1"/>
+    </row>
+    <row r="887" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B887" s="1"/>
+    </row>
+    <row r="888" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B888" s="1"/>
+    </row>
+    <row r="889" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B889" s="1"/>
+    </row>
+    <row r="890" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B890" s="1"/>
+    </row>
+    <row r="891" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B891" s="1"/>
+    </row>
+    <row r="892" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B892" s="1"/>
+    </row>
+    <row r="893" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B893" s="1"/>
+    </row>
+    <row r="894" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B894" s="1"/>
+    </row>
+    <row r="895" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B895" s="1"/>
+    </row>
+    <row r="896" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B896" s="1"/>
+    </row>
+    <row r="897" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B897" s="1"/>
+    </row>
+    <row r="898" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B898" s="1"/>
+    </row>
+    <row r="899" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B899" s="1"/>
+    </row>
+    <row r="900" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B900" s="1"/>
+    </row>
+    <row r="901" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B901" s="1"/>
+    </row>
+    <row r="902" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B902" s="1"/>
+    </row>
+    <row r="903" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B903" s="1"/>
+    </row>
+    <row r="904" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B904" s="1"/>
+    </row>
+    <row r="905" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B905" s="1"/>
+    </row>
+    <row r="906" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B906" s="1"/>
+    </row>
+    <row r="907" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B907" s="1"/>
+    </row>
+    <row r="908" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B908" s="1"/>
+    </row>
+    <row r="909" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B909" s="1"/>
+    </row>
+    <row r="910" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B910" s="1"/>
+    </row>
+    <row r="911" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B911" s="1"/>
+    </row>
+    <row r="912" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B912" s="1"/>
+    </row>
+    <row r="913" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B913" s="1"/>
+    </row>
+    <row r="914" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B914" s="1"/>
+    </row>
+    <row r="915" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B915" s="1"/>
+    </row>
+    <row r="916" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B916" s="1"/>
+    </row>
+    <row r="917" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B917" s="1"/>
+    </row>
+    <row r="918" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B918" s="1"/>
+    </row>
+    <row r="919" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B919" s="1"/>
+    </row>
+    <row r="920" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B920" s="1"/>
+    </row>
+    <row r="921" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B921" s="1"/>
+    </row>
+    <row r="922" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B922" s="1"/>
+    </row>
+    <row r="923" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B923" s="1"/>
+    </row>
+    <row r="924" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B924" s="1"/>
+    </row>
+    <row r="925" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B925" s="1"/>
+    </row>
+    <row r="926" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B926" s="1"/>
+    </row>
+    <row r="927" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B927" s="1"/>
+    </row>
+    <row r="928" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B928" s="1"/>
+    </row>
+    <row r="929" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B929" s="1"/>
+    </row>
+    <row r="930" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B930" s="1"/>
+    </row>
+    <row r="931" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B931" s="1"/>
+    </row>
+    <row r="932" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B932" s="1"/>
+    </row>
+    <row r="933" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B933" s="1"/>
+    </row>
+    <row r="934" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B934" s="1"/>
+    </row>
+    <row r="935" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B935" s="1"/>
+    </row>
+    <row r="936" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B936" s="1"/>
+    </row>
+    <row r="937" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B937" s="1"/>
+    </row>
+    <row r="938" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B938" s="1"/>
+    </row>
+    <row r="939" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B939" s="1"/>
+    </row>
+    <row r="940" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B940" s="1"/>
+    </row>
+    <row r="941" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B941" s="1"/>
+    </row>
+    <row r="942" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B942" s="1"/>
+    </row>
+    <row r="943" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B943" s="1"/>
+    </row>
+    <row r="944" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B944" s="1"/>
+    </row>
+    <row r="945" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B945" s="1"/>
+    </row>
+    <row r="946" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B946" s="1"/>
+    </row>
+    <row r="947" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B947" s="1"/>
+    </row>
+    <row r="948" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B948" s="1"/>
+    </row>
+    <row r="949" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B949" s="1"/>
+    </row>
+    <row r="950" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B950" s="1"/>
+    </row>
+    <row r="951" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B951" s="1"/>
+    </row>
+    <row r="952" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B952" s="1"/>
+    </row>
+    <row r="953" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B953" s="1"/>
+    </row>
+    <row r="954" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B954" s="1"/>
+    </row>
+    <row r="955" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B955" s="1"/>
+    </row>
+    <row r="956" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B956" s="1"/>
+    </row>
+    <row r="957" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B957" s="1"/>
+    </row>
+    <row r="958" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B958" s="1"/>
+    </row>
+    <row r="959" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B959" s="1"/>
+    </row>
+    <row r="960" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B960" s="1"/>
+    </row>
+    <row r="961" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B961" s="1"/>
+    </row>
+    <row r="962" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B962" s="1"/>
+    </row>
+    <row r="963" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B963" s="1"/>
+    </row>
+    <row r="964" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B964" s="1"/>
+    </row>
+    <row r="965" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B965" s="1"/>
+    </row>
+    <row r="966" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B966" s="1"/>
+    </row>
+    <row r="967" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B967" s="1"/>
+    </row>
+    <row r="968" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B968" s="1"/>
+    </row>
+    <row r="969" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B969" s="1"/>
+    </row>
+    <row r="970" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B970" s="1"/>
+    </row>
+    <row r="971" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B971" s="1"/>
+    </row>
+    <row r="972" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B972" s="1"/>
+    </row>
+    <row r="973" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B973" s="1"/>
+    </row>
+    <row r="974" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B974" s="1"/>
+    </row>
+    <row r="975" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B975" s="1"/>
+    </row>
+    <row r="976" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B976" s="1"/>
+    </row>
+    <row r="977" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B977" s="1"/>
+    </row>
+    <row r="978" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B978" s="1"/>
+    </row>
+    <row r="979" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B979" s="1"/>
+    </row>
+    <row r="980" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B980" s="1"/>
+    </row>
+    <row r="981" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B981" s="1"/>
+    </row>
+    <row r="982" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B982" s="1"/>
+    </row>
+    <row r="983" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B983" s="1"/>
+    </row>
+    <row r="984" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B984" s="1"/>
+    </row>
+    <row r="985" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B985" s="1"/>
+    </row>
+    <row r="986" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B986" s="1"/>
+    </row>
+    <row r="987" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B987" s="1"/>
+    </row>
+    <row r="988" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B988" s="1"/>
+    </row>
+    <row r="989" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B989" s="1"/>
+    </row>
+    <row r="990" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B990" s="1"/>
+    </row>
+    <row r="991" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B991" s="1"/>
+    </row>
+    <row r="992" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B992" s="1"/>
+    </row>
+    <row r="993" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B993" s="1"/>
+    </row>
+    <row r="994" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B994" s="1"/>
+    </row>
+    <row r="995" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B995" s="1"/>
+    </row>
+    <row r="996" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B996" s="1"/>
+    </row>
+    <row r="997" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B997" s="1"/>
+    </row>
+    <row r="998" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B998" s="1"/>
+    </row>
+    <row r="999" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B999" s="1"/>
+    </row>
+    <row r="1000" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1000" s="1"/>
+    </row>
+    <row r="1001" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1001" s="1"/>
+    </row>
+    <row r="1002" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1002" s="1"/>
+    </row>
+    <row r="1003" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1003" s="1"/>
+    </row>
+    <row r="1004" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1004" s="1"/>
+    </row>
+    <row r="1005" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1005" s="1"/>
+    </row>
+    <row r="1006" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1006" s="1"/>
+    </row>
+    <row r="1007" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1007" s="1"/>
+    </row>
+    <row r="1008" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1008" s="1"/>
+    </row>
+    <row r="1009" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1009" s="1"/>
+    </row>
+    <row r="1010" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1010" s="1"/>
+    </row>
+    <row r="1011" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1011" s="1"/>
+    </row>
+    <row r="1012" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1012" s="1"/>
+    </row>
+    <row r="1013" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1013" s="1"/>
+    </row>
+    <row r="1014" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1014" s="1"/>
+    </row>
+    <row r="1015" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1015" s="1"/>
+    </row>
+    <row r="1016" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1016" s="1"/>
+    </row>
+    <row r="1017" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1017" s="1"/>
+    </row>
+    <row r="1018" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1018" s="1"/>
+    </row>
+    <row r="1019" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1019" s="1"/>
+    </row>
+    <row r="1020" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1020" s="1"/>
+    </row>
+    <row r="1021" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1021" s="1"/>
+    </row>
+    <row r="1022" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1022" s="1"/>
+    </row>
+    <row r="1023" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1023" s="1"/>
+    </row>
+    <row r="1024" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1024" s="1"/>
+    </row>
+    <row r="1025" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1025" s="1"/>
+    </row>
+    <row r="1026" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1026" s="1"/>
+    </row>
+    <row r="1027" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1027" s="1"/>
+    </row>
+    <row r="1028" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1028" s="1"/>
+    </row>
+    <row r="1029" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1029" s="1"/>
+    </row>
+    <row r="1030" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1030" s="1"/>
+    </row>
+    <row r="1031" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1031" s="1"/>
+    </row>
+    <row r="1032" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1032" s="1"/>
+    </row>
+    <row r="1033" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1033" s="1"/>
+    </row>
+    <row r="1034" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1034" s="1"/>
+    </row>
+    <row r="1035" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1035" s="1"/>
+    </row>
+    <row r="1036" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1036" s="1"/>
+    </row>
+    <row r="1037" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1037" s="1"/>
+    </row>
+    <row r="1038" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1038" s="1"/>
+    </row>
+    <row r="1039" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1039" s="1"/>
+    </row>
+    <row r="1040" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1040" s="1"/>
+    </row>
+    <row r="1041" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1041" s="1"/>
+    </row>
+    <row r="1042" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1042" s="1"/>
+    </row>
+    <row r="1043" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1043" s="1"/>
+    </row>
+    <row r="1044" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1044" s="1"/>
+    </row>
+    <row r="1045" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1045" s="1"/>
+    </row>
+    <row r="1046" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1046" s="1"/>
+    </row>
+    <row r="1047" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1047" s="1"/>
+    </row>
+    <row r="1048" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1048" s="1"/>
+    </row>
+    <row r="1049" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1049" s="1"/>
+    </row>
+    <row r="1050" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1050" s="1"/>
+    </row>
+    <row r="1051" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1051" s="1"/>
+    </row>
+    <row r="1052" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1052" s="1"/>
+    </row>
+    <row r="1053" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1053" s="1"/>
+    </row>
+    <row r="1054" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1054" s="1"/>
+    </row>
+    <row r="1055" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1055" s="1"/>
+    </row>
+    <row r="1056" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1056" s="1"/>
+    </row>
+    <row r="1057" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1057" s="1"/>
+    </row>
+    <row r="1058" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1058" s="1"/>
+    </row>
+    <row r="1059" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1059" s="1"/>
+    </row>
+    <row r="1060" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1060" s="1"/>
+    </row>
+    <row r="1061" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1061" s="1"/>
+    </row>
+    <row r="1062" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1062" s="1"/>
+    </row>
+    <row r="1063" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1063" s="1"/>
+    </row>
+    <row r="1064" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1064" s="1"/>
+    </row>
+    <row r="1065" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1065" s="1"/>
+    </row>
+    <row r="1066" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1066" s="1"/>
+    </row>
+    <row r="1067" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1067" s="1"/>
+    </row>
+    <row r="1068" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1068" s="1"/>
+    </row>
+    <row r="1069" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1069" s="1"/>
+    </row>
+    <row r="1070" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1070" s="1"/>
+    </row>
+    <row r="1071" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1071" s="1"/>
+    </row>
+    <row r="1072" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1072" s="1"/>
+    </row>
+    <row r="1073" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1073" s="1"/>
+    </row>
+    <row r="1074" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1074" s="1"/>
+    </row>
+    <row r="1075" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1075" s="1"/>
+    </row>
+    <row r="1076" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1076" s="1"/>
+    </row>
+    <row r="1077" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1077" s="1"/>
+    </row>
+    <row r="1078" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1078" s="1"/>
+    </row>
+    <row r="1079" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1079" s="1"/>
+    </row>
+    <row r="1080" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1080" s="1"/>
+    </row>
+    <row r="1081" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1081" s="1"/>
+    </row>
+    <row r="1082" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1082" s="1"/>
+    </row>
+    <row r="1083" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1083" s="1"/>
+    </row>
+    <row r="1084" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1084" s="1"/>
+    </row>
+    <row r="1085" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1085" s="1"/>
+    </row>
+    <row r="1086" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1086" s="1"/>
+    </row>
+    <row r="1087" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1087" s="1"/>
+    </row>
+    <row r="1088" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1088" s="1"/>
+    </row>
+    <row r="1089" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1089" s="1"/>
+    </row>
+    <row r="1090" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1090" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ABM preguntas back-end e interfaz de usuario administrador
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="78">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t>Análisis de Base de Datos y UML para incorporación de Sprint</t>
+  </si>
+  <si>
+    <t>Sprint 4 - Preguntas</t>
+  </si>
+  <si>
+    <t>Creación de Back-end, Preguntas back e I.U. Administrador (ABM preguntas)</t>
   </si>
 </sst>
 </file>
@@ -601,7 +607,7 @@
   <dimension ref="A1:E1091"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1859,7 +1865,21 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B75" s="1"/>
+      <c r="A75" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="1">
+        <v>42900</v>
+      </c>
+      <c r="C75">
+        <v>4</v>
+      </c>
+      <c r="D75" t="s">
+        <v>76</v>
+      </c>
+      <c r="E75" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B76" s="1"/>

</xml_diff>

<commit_message>
Prueba de entorno de producción
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="86">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -265,6 +265,18 @@
   </si>
   <si>
     <t>Sprint 5 - Documentación</t>
+  </si>
+  <si>
+    <t>Solucionando problemas para poder correr frontEnd</t>
+  </si>
+  <si>
+    <t>Solucionando problemas con el IDE</t>
+  </si>
+  <si>
+    <t>Investigando para Hostear todo</t>
+  </si>
+  <si>
+    <t>Se pasó la conexión al WebConfig, se probó que ande, se creó la base spods en GoDaddy, se probó que me pueda conectar a esa.</t>
   </si>
 </sst>
 </file>
@@ -603,7 +615,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -613,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1091"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1940,10 +1952,38 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B79" s="1"/>
+      <c r="A79" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79" s="1">
+        <v>42902</v>
+      </c>
+      <c r="C79">
+        <v>4</v>
+      </c>
+      <c r="D79" t="s">
+        <v>83</v>
+      </c>
+      <c r="E79" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B80" s="1"/>
+      <c r="A80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" s="1">
+        <v>42902</v>
+      </c>
+      <c r="C80">
+        <v>4</v>
+      </c>
+      <c r="D80" t="s">
+        <v>84</v>
+      </c>
+      <c r="E80" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="1"/>

</xml_diff>

<commit_message>
Trabajando en Back-en Servicios e IU administrador.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="88">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -277,6 +282,12 @@
   </si>
   <si>
     <t>Se pasó la conexión al WebConfig, se probó que ande, se creó la base spods en GoDaddy, se probó que me pueda conectar a esa.</t>
+  </si>
+  <si>
+    <t>Sprint 4 - Servicios</t>
+  </si>
+  <si>
+    <t>Creación de Back-end, Servicios back e I.U. Administrador (ABM servicios)</t>
   </si>
 </sst>
 </file>
@@ -615,7 +626,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -626,7 +637,7 @@
   <dimension ref="A1:E1091"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1985,52 +1996,66 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B81" s="1"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81" s="1">
+        <v>42903</v>
+      </c>
+      <c r="C81">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
+        <v>86</v>
+      </c>
+      <c r="E81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B84" s="1"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B85" s="1"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B86" s="1"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B87" s="1"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B88" s="1"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B89" s="1"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B96" s="1"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Back-end e IU Administrador pronto. Servicio para obtener todos los servicios habilitados pronto.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="89">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>Creación de Back-end, Servicios back e I.U. Administrador (ABM servicios)</t>
+  </si>
+  <si>
+    <t>Imagenes, Servicio para obtener todos los servicios habilitados</t>
   </si>
 </sst>
 </file>
@@ -637,7 +640,7 @@
   <dimension ref="A1:E1091"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2014,7 +2017,21 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B82" s="1"/>
+      <c r="A82" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" s="1">
+        <v>42904</v>
+      </c>
+      <c r="C82">
+        <v>3</v>
+      </c>
+      <c r="D82" t="s">
+        <v>86</v>
+      </c>
+      <c r="E82" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B83" s="1"/>

</xml_diff>

<commit_message>
Cambio en gitIgnore (se sacó la carpeta packages). Se arregló el problema en el package.json para poder hacer el install. Carga de horas de lo hecho el finde.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="93">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -291,6 +286,18 @@
   </si>
   <si>
     <t>Imagenes, Servicio para obtener todos los servicios habilitados</t>
+  </si>
+  <si>
+    <t>Se pudo alojar el Backend y el proyecto que brinda los servicios. Se investigó sobre cómo subir el front</t>
+  </si>
+  <si>
+    <t>Se investigó sobre cómo subir el front</t>
+  </si>
+  <si>
+    <t>Solucionando problema de versiones</t>
+  </si>
+  <si>
+    <t>Se solucionó concretamente el problema de la versión que estaba cargando algún archivo mal… Se puede hacer el install sin problemas</t>
   </si>
 </sst>
 </file>
@@ -629,7 +636,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -637,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1091"/>
+  <dimension ref="A1:E1092"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2018,29 +2025,71 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B82" s="1">
+        <v>42903</v>
+      </c>
+      <c r="C82">
+        <v>9</v>
+      </c>
+      <c r="D82" t="s">
+        <v>84</v>
+      </c>
+      <c r="E82" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83" s="1">
         <v>42904</v>
       </c>
-      <c r="C82">
+      <c r="C83">
         <v>3</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D83" t="s">
         <v>86</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E83" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B83" s="1"/>
-    </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B84" s="1"/>
+      <c r="A84" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" s="1">
+        <v>42904</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>84</v>
+      </c>
+      <c r="E84" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B85" s="1"/>
+      <c r="A85" t="s">
+        <v>18</v>
+      </c>
+      <c r="B85" s="1">
+        <v>42904</v>
+      </c>
+      <c r="C85">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s">
+        <v>91</v>
+      </c>
+      <c r="E85" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B86" s="1"/>
@@ -5059,6 +5108,9 @@
     </row>
     <row r="1091" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B1091" s="1"/>
+    </row>
+    <row r="1092" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1092" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Diagrama de clases, Mer, Base de datos y estructira Back-end. Falta construir clase comentariosPuntuacion en capa ET. Capa DAL de Publicacion incompleta.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="97">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -309,6 +309,12 @@
   </si>
   <si>
     <t>Documentación de los sprints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 5 </t>
+  </si>
+  <si>
+    <t>Diagrama de clases, Mer, Base de datos y estructura del Backend</t>
   </si>
 </sst>
 </file>
@@ -658,7 +664,7 @@
   <dimension ref="A1:E1092"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2137,7 +2143,21 @@
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B88" s="1"/>
+      <c r="A88" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="1">
+        <v>42910</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88" t="s">
+        <v>95</v>
+      </c>
+      <c r="E88" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B89" s="1"/>

</xml_diff>

<commit_message>
Back-end, web api, algunos test para probar funcionalidades de sprint 5.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="100">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -315,6 +315,15 @@
   </si>
   <si>
     <t>Diagrama de clases, Mer, Base de datos y estructura del Backend</t>
+  </si>
+  <si>
+    <t>Back-end capas et, bl, dal.</t>
+  </si>
+  <si>
+    <t>Back-end web api, algunos test para probar funcionalidades</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
   </si>
 </sst>
 </file>
@@ -663,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1092"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2160,10 +2169,38 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B89" s="1"/>
+      <c r="A89" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89" s="1">
+        <v>42911</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+      <c r="D89" t="s">
+        <v>99</v>
+      </c>
+      <c r="E89" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B90" s="1"/>
+      <c r="A90" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90" s="1">
+        <v>42912</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="D90" t="s">
+        <v>99</v>
+      </c>
+      <c r="E90" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B91" s="1"/>

</xml_diff>

<commit_message>
Back-end publicaciones casi pronto. Respuestas agregadas a  la publicacion.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="101">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Back-end web api, algunos test para probar funcionalidades. Respuestas a preguntas de la publicaci'on.</t>
   </si>
 </sst>
 </file>
@@ -672,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1092"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2203,7 +2206,21 @@
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B91" s="1"/>
+      <c r="A91" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91" s="1">
+        <v>42914</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91" t="s">
+        <v>99</v>
+      </c>
+      <c r="E91" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B92" s="1"/>

</xml_diff>

<commit_message>
Front-end cliente, Listado de publicaciones de un cliente, activar/desactivar publicacion, editar publicacion
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="6792"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="106">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -331,6 +336,12 @@
   </si>
   <si>
     <t>Documentación de Sprint 3</t>
+  </si>
+  <si>
+    <t>Front-end cliente alta publicaci'on</t>
+  </si>
+  <si>
+    <t>Front-end cliente Listado publicaciones cliente, habilitar-deshabilitar, editar publicacion</t>
   </si>
 </sst>
 </file>
@@ -669,7 +680,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -680,7 +691,7 @@
   <dimension ref="A1:E1098"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2431,10 +2442,38 @@
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B104" s="1"/>
+      <c r="A104" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104" s="1">
+        <v>42918</v>
+      </c>
+      <c r="C104">
+        <v>6</v>
+      </c>
+      <c r="D104" t="s">
+        <v>98</v>
+      </c>
+      <c r="E104" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B105" s="1"/>
+      <c r="A105" t="s">
+        <v>4</v>
+      </c>
+      <c r="B105" s="1">
+        <v>42919</v>
+      </c>
+      <c r="C105">
+        <v>6</v>
+      </c>
+      <c r="D105" t="s">
+        <v>98</v>
+      </c>
+      <c r="E105" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B106" s="1"/>

</xml_diff>

<commit_message>
Arreglos en el front Sprint 5, Listado con las publicaciones por servicio.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="107">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>Front-end cliente Listado publicaciones cliente, habilitar-deshabilitar, editar publicacion</t>
+  </si>
+  <si>
+    <t>Front-end cliente editar publicacion, Listado de las publicaciones por servicio.</t>
   </si>
 </sst>
 </file>
@@ -690,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1098"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="B72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2476,10 +2479,38 @@
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B106" s="1"/>
+      <c r="A106" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106" s="1">
+        <v>42920</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s">
+        <v>98</v>
+      </c>
+      <c r="E106" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B107" s="1"/>
+      <c r="A107" t="s">
+        <v>4</v>
+      </c>
+      <c r="B107" s="1">
+        <v>42925</v>
+      </c>
+      <c r="C107">
+        <v>6</v>
+      </c>
+      <c r="D107" t="s">
+        <v>98</v>
+      </c>
+      <c r="E107" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B108" s="1"/>

</xml_diff>

<commit_message>
Subida de imagenes con Iframe
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="108">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t>Front-end cliente editar publicacion, Listado de las publicaciones por servicio.</t>
+  </si>
+  <si>
+    <t>Front-end cliente subida de imagenes desde angular, resgitro cliente.</t>
   </si>
 </sst>
 </file>
@@ -693,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1098"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" topLeftCell="B93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2513,7 +2516,18 @@
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B108" s="1"/>
+      <c r="B108" s="1">
+        <v>42926</v>
+      </c>
+      <c r="C108">
+        <v>10</v>
+      </c>
+      <c r="D108" t="s">
+        <v>98</v>
+      </c>
+      <c r="E108" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B109" s="1"/>

</xml_diff>

<commit_message>
Registro clientes en pasos con imagenes
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="110">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t>Front-end cliente subida de imagenes desde angular, resgitro cliente.</t>
+  </si>
+  <si>
+    <t>Imagenes cliente front</t>
+  </si>
+  <si>
+    <t>Registro cliente con imagenes y en pasos</t>
   </si>
 </sst>
 </file>
@@ -696,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1098"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2516,6 +2522,9 @@
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>4</v>
+      </c>
       <c r="B108" s="1">
         <v>42926</v>
       </c>
@@ -2530,10 +2539,38 @@
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B109" s="1"/>
+      <c r="A109" t="s">
+        <v>4</v>
+      </c>
+      <c r="B109" s="1">
+        <v>42927</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109" t="s">
+        <v>98</v>
+      </c>
+      <c r="E109" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B110" s="1"/>
+      <c r="A110" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110" s="1">
+        <v>42928</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s">
+        <v>98</v>
+      </c>
+      <c r="E110" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B111" s="1"/>

</xml_diff>

<commit_message>
Oferta y editar oferta con imagenes, back y front casi pronto
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="112">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t>Registro cliente con imagenes y en pasos</t>
+  </si>
+  <si>
+    <t>Sprint 6</t>
+  </si>
+  <si>
+    <t>Imagenes publicacion oferta, back y front</t>
   </si>
 </sst>
 </file>
@@ -703,7 +709,7 @@
   <dimension ref="A1:E1098"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2573,7 +2579,21 @@
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B111" s="1"/>
+      <c r="A111" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" s="1">
+        <v>42932</v>
+      </c>
+      <c r="C111">
+        <v>10</v>
+      </c>
+      <c r="D111" t="s">
+        <v>110</v>
+      </c>
+      <c r="E111" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B112" s="1"/>

</xml_diff>

<commit_message>
Alta de comentario desde el front... quedan detalles.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="114">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>Imagenes publicacion oferta, back y front</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comentarios y puntuación. </t>
+  </si>
+  <si>
+    <t>Comentarios y puntuación. Algunos retoques para subir el proyecto.</t>
   </si>
 </sst>
 </file>
@@ -709,7 +715,7 @@
   <dimension ref="A1:E1098"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+      <selection activeCell="E113" sqref="E113:E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2596,54 +2602,96 @@
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B112" s="1"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B113" s="1"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B114" s="1"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112" s="1">
+        <v>42939</v>
+      </c>
+      <c r="C112">
+        <v>9</v>
+      </c>
+      <c r="D112" t="s">
+        <v>110</v>
+      </c>
+      <c r="E112" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113" s="1">
+        <v>42940</v>
+      </c>
+      <c r="C113">
+        <v>9</v>
+      </c>
+      <c r="D113" t="s">
+        <v>110</v>
+      </c>
+      <c r="E113" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>4</v>
+      </c>
+      <c r="B114" s="1">
+        <v>42942</v>
+      </c>
+      <c r="C114">
+        <v>2</v>
+      </c>
+      <c r="D114" t="s">
+        <v>110</v>
+      </c>
+      <c r="E114" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B115" s="1"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B116" s="1"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B117" s="1"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B118" s="1"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B119" s="1"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B120" s="1"/>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B121" s="1"/>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B122" s="1"/>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B123" s="1"/>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B124" s="1"/>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B125" s="1"/>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B126" s="1"/>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B127" s="1"/>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B128" s="1"/>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Comentario y puntuaje terminados para las ofertas laborales.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="115">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>Comentarios y puntuación. Algunos retoques para subir el proyecto.</t>
+  </si>
+  <si>
+    <t>Comentario y puntuacion. Respuestas y promedios.</t>
   </si>
 </sst>
 </file>
@@ -401,9 +404,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1098"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113:E114"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2648,15 +2652,43 @@
       <c r="D114" t="s">
         <v>110</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B115" s="1"/>
+      <c r="A115" t="s">
+        <v>4</v>
+      </c>
+      <c r="B115" s="1">
+        <v>42946</v>
+      </c>
+      <c r="C115">
+        <v>10</v>
+      </c>
+      <c r="D115" t="s">
+        <v>110</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B116" s="1"/>
+      <c r="A116" t="s">
+        <v>4</v>
+      </c>
+      <c r="B116" s="1">
+        <v>42950</v>
+      </c>
+      <c r="C116">
+        <v>5</v>
+      </c>
+      <c r="D116" t="s">
+        <v>110</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B117" s="1"/>

</xml_diff>

<commit_message>
Arreglos en front y back, publicacion.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="120">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -378,6 +378,12 @@
   </si>
   <si>
     <t>Alta presupuesto, listado de presupuestos.</t>
+  </si>
+  <si>
+    <t>Aceptar presupuesto back y front</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arreglos en publicacion, cambios en la base tabla publicacion, arreglo de todas las consultas, cambios en el front. </t>
   </si>
 </sst>
 </file>
@@ -728,7 +734,7 @@
   <dimension ref="A1:E1098"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A105" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+      <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2734,10 +2740,38 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B119" s="1"/>
+      <c r="A119" t="s">
+        <v>4</v>
+      </c>
+      <c r="B119" s="1">
+        <v>42955</v>
+      </c>
+      <c r="C119">
+        <v>6</v>
+      </c>
+      <c r="D119" t="s">
+        <v>115</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B120" s="1"/>
+      <c r="A120" t="s">
+        <v>4</v>
+      </c>
+      <c r="B120" s="1">
+        <v>42956</v>
+      </c>
+      <c r="C120">
+        <v>6</v>
+      </c>
+      <c r="D120" t="s">
+        <v>115</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B121" s="1"/>

</xml_diff>

<commit_message>
Arreglos en comentario y aceptar propuesta. Queda pendiente comentar una solicitud, mostrar todos los tipos de puntajes y armar un buen perfil de usuario para mostrar los datos.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="121">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t xml:space="preserve">Arreglos en publicacion, cambios en la base tabla publicacion, arreglo de todas las consultas, cambios en el front. </t>
+  </si>
+  <si>
+    <t>Arreglos en comentarios y aceptar propuesta.</t>
   </si>
 </sst>
 </file>
@@ -733,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1098"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2774,7 +2777,21 @@
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B121" s="1"/>
+      <c r="A121" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121" s="1">
+        <v>42958</v>
+      </c>
+      <c r="C121">
+        <v>4</v>
+      </c>
+      <c r="D121" t="s">
+        <v>115</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B122" s="1"/>

</xml_diff>

<commit_message>
Testing y arreglos. Front.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="122">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>Arreglos en comentarios y aceptar propuesta.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing Front. </t>
   </si>
 </sst>
 </file>
@@ -736,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1098"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2794,13 +2797,55 @@
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B122" s="1"/>
+      <c r="A122" t="s">
+        <v>4</v>
+      </c>
+      <c r="B122" s="1">
+        <v>42966</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="D122" t="s">
+        <v>115</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B123" s="1"/>
+      <c r="A123" t="s">
+        <v>4</v>
+      </c>
+      <c r="B123" s="1">
+        <v>42967</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
+      <c r="D123" t="s">
+        <v>115</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B124" s="1"/>
+      <c r="A124" t="s">
+        <v>4</v>
+      </c>
+      <c r="B124" s="1">
+        <v>42968</v>
+      </c>
+      <c r="C124">
+        <v>4</v>
+      </c>
+      <c r="D124" t="s">
+        <v>115</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B125" s="1"/>

</xml_diff>

<commit_message>
Arreglos en Front y Back de la lista realizada en el testing.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="123">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -389,7 +389,10 @@
     <t>Arreglos en comentarios y aceptar propuesta.</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing Front. </t>
+    <t>Arreglos y faltantes en front y back.</t>
+  </si>
+  <si>
+    <t>Testing Front. Listado con faltantes y arreglos.</t>
   </si>
 </sst>
 </file>
@@ -740,7 +743,7 @@
   <dimension ref="A1:E1098"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+      <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2844,7 +2847,7 @@
         <v>115</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2861,11 +2864,25 @@
         <v>115</v>
       </c>
       <c r="E125" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>4</v>
+      </c>
+      <c r="B126" s="1">
+        <v>42975</v>
+      </c>
+      <c r="C126">
+        <v>9</v>
+      </c>
+      <c r="D126" t="s">
+        <v>115</v>
+      </c>
+      <c r="E126" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B126" s="1"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B127" s="1"/>

</xml_diff>

<commit_message>
Arreglos, se crea la clase oferta con puntaje y cantidad de comentarios. Se muestran los datos en el listado de publicaciones ofrecidas por servicio.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="125">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -393,6 +393,12 @@
   </si>
   <si>
     <t>Testing Front. Listado con faltantes y arreglos.</t>
+  </si>
+  <si>
+    <t>Sprint 8</t>
+  </si>
+  <si>
+    <t>Arreglos del listado de faltantes, se crea la clase oferta con puntaje y cantidad de comentarios, retoque en servicios, se muestra puntaje y cantidad de comentarios en el listado.</t>
   </si>
 </sst>
 </file>
@@ -743,7 +749,7 @@
   <dimension ref="A1:E1098"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E125" sqref="E125"/>
+      <selection activeCell="E127" sqref="E126:E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2885,7 +2891,21 @@
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B127" s="1"/>
+      <c r="A127" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127" s="1">
+        <v>42980</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="D127" t="s">
+        <v>123</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B128" s="1"/>

</xml_diff>

<commit_message>
Detalles de la lista de faltantes.
</commit_message>
<xml_diff>
--- a/Documentacion/Horas.xlsx
+++ b/Documentacion/Horas.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="127">
   <si>
     <t>Horas trabajadas</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>Arreglos, puntajes.</t>
+  </si>
+  <si>
+    <t>Detalles de la lista de faltantes.</t>
   </si>
 </sst>
 </file>
@@ -751,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1098"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2927,52 +2930,66 @@
         <v>125</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B129" s="1"/>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>4</v>
+      </c>
+      <c r="B129" s="1">
+        <v>42984</v>
+      </c>
+      <c r="C129">
+        <v>5</v>
+      </c>
+      <c r="D129" t="s">
+        <v>123</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B130" s="1"/>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B131" s="1"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B132" s="1"/>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B133" s="1"/>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B134" s="1"/>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B135" s="1"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B136" s="1"/>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B137" s="1"/>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B138" s="1"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B139" s="1"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B140" s="1"/>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B141" s="1"/>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B142" s="1"/>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B143" s="1"/>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B144" s="1"/>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>